<commit_message>
Mise en place cout assemblages
</commit_message>
<xml_diff>
--- a/CR - Cost Report/CBOM/Materials_cost.xlsx
+++ b/CR - Cost Report/CBOM/Materials_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid" sheetId="4" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="B9:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>